<commit_message>
before thesis committee update
</commit_message>
<xml_diff>
--- a/Pleth_Breath_Types/Currently_labeling_data/Unseen (Blinded)/rat23466_unseen_data_clean_type2.xlsx
+++ b/Pleth_Breath_Types/Currently_labeling_data/Unseen (Blinded)/rat23466_unseen_data_clean_type2.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="365" uniqueCount="283">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="366" uniqueCount="286">
   <si>
     <t>Sample</t>
   </si>
@@ -864,10 +864,19 @@
     <t xml:space="preserve">f </t>
   </si>
   <si>
-    <t>KEY: Quiet Breathing (0), Sigh (1), Sniffing (2), Apnea (3)</t>
-  </si>
-  <si>
     <t>type II too</t>
+  </si>
+  <si>
+    <t>maybe type II too</t>
+  </si>
+  <si>
+    <t>type II too, limit</t>
+  </si>
+  <si>
+    <t>KEY: Quiet Breathing (0), Sigh (1), Sniffing (2), Random Apnea (3), Type II Apnea (4)</t>
+  </si>
+  <si>
+    <t>type II too, limit, maybe switch</t>
   </si>
 </sst>
 </file>
@@ -1282,9 +1291,9 @@
   <dimension ref="A1:AJ81"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A50" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="K1" sqref="K1"/>
-      <selection pane="bottomLeft" activeCell="AH77" sqref="AH77"/>
+      <selection pane="bottomLeft" activeCell="AH42" sqref="AH42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1403,7 +1412,7 @@
         <v>280</v>
       </c>
       <c r="AJ1" s="5" t="s">
-        <v>281</v>
+        <v>284</v>
       </c>
     </row>
     <row r="2" spans="1:36" x14ac:dyDescent="0.25">
@@ -3587,7 +3596,7 @@
         <v>4</v>
       </c>
       <c r="AH22" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="AI22" s="7">
         <v>12</v>
@@ -3694,7 +3703,7 @@
         <v>4</v>
       </c>
       <c r="AH23" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="AI23" s="7">
         <v>29</v>
@@ -3801,7 +3810,7 @@
         <v>4</v>
       </c>
       <c r="AH24" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="AI24" s="7">
         <v>30</v>
@@ -3908,7 +3917,7 @@
         <v>4</v>
       </c>
       <c r="AH25" t="s">
-        <v>282</v>
+        <v>285</v>
       </c>
       <c r="AI25" s="7">
         <v>32</v>
@@ -4014,6 +4023,9 @@
       <c r="AG26" s="9">
         <v>1</v>
       </c>
+      <c r="AH26" t="s">
+        <v>282</v>
+      </c>
       <c r="AI26" s="7">
         <v>35</v>
       </c>
@@ -4116,7 +4128,7 @@
         <v>3477</v>
       </c>
       <c r="AG27" s="9">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="AH27" t="s">
         <v>282</v>
@@ -4223,7 +4235,7 @@
         <v>4346</v>
       </c>
       <c r="AG28" s="9">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="AH28" t="s">
         <v>282</v>
@@ -4330,7 +4342,7 @@
         <v>6589</v>
       </c>
       <c r="AG29" s="9">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="AH29" t="s">
         <v>282</v>
@@ -4437,7 +4449,7 @@
         <v>3991</v>
       </c>
       <c r="AG30" s="9">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="AH30" t="s">
         <v>282</v>
@@ -4544,7 +4556,7 @@
         <v>9199</v>
       </c>
       <c r="AG31" s="9">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="AH31" t="s">
         <v>282</v>

</xml_diff>